<commit_message>
implemented ordered execution, but not working as expected
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t/>
   </si>
@@ -21,6 +22,21 @@
   </si>
   <si>
     <t>Mobile</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>dine</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>raj</t>
   </si>
 </sst>
 </file>
@@ -92,5 +108,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>